<commit_message>
feat: update xlsx imports
</commit_message>
<xml_diff>
--- a/database/seeders/enderecos/xlsx/bairros/seed_bairros_itarare.xlsx
+++ b/database/seeders/enderecos/xlsx/bairros/seed_bairros_itarare.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maia/Documents/Projetos/gcm/backend/src/shared/infra/typeorm/seeds/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmaia/Documents/Dev/sysgcm/database/seeders/enderecos/xlsx/bairros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C469DAFA-9326-4BA9-B1A8-4EFCB8EAF576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4269B8-8AFF-F140-8C7C-1251157C1A36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13860" xr2:uid="{E47AA242-32C8-4F40-AE81-9A7D90E6F8BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13680" xr2:uid="{E47AA242-32C8-4F40-AE81-9A7D90E6F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -559,7 +559,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -911,20 +911,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A40675-F120-C64E-96B3-624AD610153C}">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:E104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.125" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -943,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -951,7 +951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -959,7 +959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -967,7 +967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -975,7 +975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -991,7 +991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -999,7 +999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>73</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>75</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>77</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>87</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>91</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>93</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>97</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>103</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>105</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>107</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>109</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>111</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>113</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>115</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>117</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>119</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>121</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>123</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>125</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>127</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>129</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>131</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>133</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>137</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>139</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>141</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>143</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>145</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>147</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>149</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>151</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>153</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>155</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>157</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>159</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>161</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>163</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>165</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>167</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>169</v>
       </c>
@@ -1607,13 +1607,67 @@
         <v>170</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B86" t="s">
         <v>172</v>
       </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat: ensure crud gcm
</commit_message>
<xml_diff>
--- a/database/seeders/enderecos/xlsx/bairros/seed_bairros_itarare.xlsx
+++ b/database/seeders/enderecos/xlsx/bairros/seed_bairros_itarare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmaia/Documents/Dev/sysgcm/database/seeders/enderecos/xlsx/bairros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4269B8-8AFF-F140-8C7C-1251157C1A36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF851D18-0947-4149-B4A8-DCF43528BE77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13680" xr2:uid="{E47AA242-32C8-4F40-AE81-9A7D90E6F8BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13660" xr2:uid="{E47AA242-32C8-4F40-AE81-9A7D90E6F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>codigo_bairro</t>
   </si>
   <si>
-    <t>nome</t>
-  </si>
-  <si>
     <t>municipio_id</t>
   </si>
   <si>
@@ -553,6 +550,9 @@
   </si>
   <si>
     <t>VILA JURANDIR</t>
+  </si>
+  <si>
+    <t>bairro</t>
   </si>
 </sst>
 </file>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A40675-F120-C64E-96B3-624AD610153C}">
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:E104"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,690 +929,690 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
         <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
         <v>57</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
         <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
         <v>61</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
         <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
         <v>65</v>
-      </c>
-      <c r="B33" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
         <v>67</v>
-      </c>
-      <c r="B34" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
         <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
         <v>71</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
         <v>73</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
         <v>75</v>
-      </c>
-      <c r="B38" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
         <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
         <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
         <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
         <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
         <v>87</v>
-      </c>
-      <c r="B44" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
         <v>89</v>
-      </c>
-      <c r="B45" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
         <v>91</v>
-      </c>
-      <c r="B46" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
         <v>93</v>
-      </c>
-      <c r="B47" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
         <v>95</v>
-      </c>
-      <c r="B48" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
         <v>97</v>
-      </c>
-      <c r="B49" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
         <v>99</v>
-      </c>
-      <c r="B50" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
         <v>101</v>
-      </c>
-      <c r="B51" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
         <v>103</v>
-      </c>
-      <c r="B52" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
         <v>105</v>
-      </c>
-      <c r="B53" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
         <v>107</v>
-      </c>
-      <c r="B54" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
         <v>109</v>
-      </c>
-      <c r="B55" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
         <v>111</v>
-      </c>
-      <c r="B56" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" t="s">
         <v>113</v>
-      </c>
-      <c r="B57" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" t="s">
         <v>115</v>
-      </c>
-      <c r="B58" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
         <v>117</v>
-      </c>
-      <c r="B59" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
         <v>119</v>
-      </c>
-      <c r="B60" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
         <v>121</v>
-      </c>
-      <c r="B61" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
         <v>123</v>
-      </c>
-      <c r="B62" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
         <v>125</v>
-      </c>
-      <c r="B63" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
         <v>127</v>
-      </c>
-      <c r="B64" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
         <v>129</v>
-      </c>
-      <c r="B65" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
         <v>131</v>
-      </c>
-      <c r="B66" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" t="s">
         <v>133</v>
-      </c>
-      <c r="B67" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
         <v>135</v>
-      </c>
-      <c r="B68" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
         <v>137</v>
-      </c>
-      <c r="B69" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
         <v>139</v>
-      </c>
-      <c r="B70" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
         <v>141</v>
-      </c>
-      <c r="B71" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
         <v>143</v>
-      </c>
-      <c r="B72" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" t="s">
         <v>145</v>
-      </c>
-      <c r="B73" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
         <v>147</v>
-      </c>
-      <c r="B74" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
         <v>149</v>
-      </c>
-      <c r="B75" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
         <v>151</v>
-      </c>
-      <c r="B76" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
         <v>153</v>
-      </c>
-      <c r="B77" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
         <v>155</v>
-      </c>
-      <c r="B78" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
         <v>157</v>
-      </c>
-      <c r="B79" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
         <v>159</v>
-      </c>
-      <c r="B80" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
         <v>161</v>
-      </c>
-      <c r="B81" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
         <v>163</v>
-      </c>
-      <c r="B82" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
         <v>165</v>
-      </c>
-      <c r="B83" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
         <v>167</v>
-      </c>
-      <c r="B84" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
         <v>169</v>
-      </c>
-      <c r="B85" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
         <v>171</v>
-      </c>
-      <c r="B86" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>